<commit_message>
SOD323 schottky switched to SOD123
Bigger means less heat issues
</commit_message>
<xml_diff>
--- a/Hardware/Alvaro-BOM.xlsx
+++ b/Hardware/Alvaro-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Alvaro\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D1AA45-CEE9-450C-9C87-B3E787E81C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70050775-F2F2-4BAE-8346-F3655374776D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="30960" windowHeight="14256" xr2:uid="{5CEEA534-026F-4018-A2AF-738414BC7216}"/>
+    <workbookView xWindow="5724" yWindow="2424" windowWidth="30960" windowHeight="14256" xr2:uid="{5CEEA534-026F-4018-A2AF-738414BC7216}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Schottky</t>
   </si>
   <si>
-    <t>SOD-323</t>
-  </si>
-  <si>
     <t>&lt;.5VF</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>16MHz</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B8:B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,10 +608,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -619,13 +619,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -633,16 +633,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -650,16 +650,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -667,16 +667,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -684,16 +684,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -701,16 +701,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
       </c>
       <c r="E12">
         <v>1</v>

</xml_diff>